<commit_message>
Added Writer to TalleyBookReaderWriter
TalleyBookReaderWriter now has a writing function that will edit the tally of 1 teacher for the specified day, period, and month.
</commit_message>
<xml_diff>
--- a/On-Call-Tracker/src/inputs/On-call_Tallies.xlsx
+++ b/On-Call-Tracker/src/inputs/On-call_Tallies.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dineth/repos/OCT-T9/On-Call-Tracker/src/inputs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -284,6 +284,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1592,22 +1593,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5" customWidth="1"/>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="4.5" style="16" customWidth="1"/>
-    <col min="4" max="7" width="4.5" style="17" customWidth="1"/>
-    <col min="8" max="8" width="4.5" style="16" customWidth="1"/>
-    <col min="9" max="12" width="4.5" style="17" customWidth="1"/>
-    <col min="13" max="13" width="4.5" style="16" customWidth="1"/>
-    <col min="14" max="17" width="4.5" style="17" customWidth="1"/>
-    <col min="18" max="18" width="4.5" style="16" customWidth="1"/>
-    <col min="19" max="23" width="4.5" style="17" customWidth="1"/>
-    <col min="24" max="24" width="8.6640625" style="18"/>
-    <col min="25" max="25" width="8.6640625" style="17"/>
-    <col min="27" max="27" width="15.33203125" customWidth="1"/>
-    <col min="28" max="28" width="8.6640625" style="1"/>
-    <col min="29" max="29" width="17.5" style="6" customWidth="1"/>
-    <col min="30" max="30" width="8.6640625" style="2"/>
+    <col min="1" max="1" customWidth="true" width="3.5"/>
+    <col min="2" max="2" customWidth="true" width="20.5"/>
+    <col min="3" max="3" customWidth="true" style="16" width="4.5"/>
+    <col min="4" max="7" customWidth="true" style="17" width="4.5"/>
+    <col min="8" max="8" customWidth="true" style="16" width="4.5"/>
+    <col min="9" max="12" customWidth="true" style="17" width="4.5"/>
+    <col min="13" max="13" customWidth="true" style="16" width="4.5"/>
+    <col min="14" max="17" customWidth="true" style="17" width="4.5"/>
+    <col min="18" max="18" customWidth="true" style="16" width="4.5"/>
+    <col min="19" max="23" customWidth="true" style="17" width="4.5"/>
+    <col min="24" max="24" style="18" width="8.6640625"/>
+    <col min="25" max="25" style="17" width="8.6640625"/>
+    <col min="27" max="27" customWidth="true" width="15.33203125"/>
+    <col min="28" max="28" style="1" width="8.6640625"/>
+    <col min="29" max="29" customWidth="true" style="6" width="17.5"/>
+    <col min="30" max="30" style="2" width="8.6640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1689,9 +1690,9 @@
       <c r="AA1" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="AB1"/>
-      <c r="AC1"/>
-      <c r="AD1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="2"/>
     </row>
     <row r="2" spans="1:30" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="50"/>
@@ -1762,9 +1763,9 @@
       <c r="Y2" s="54"/>
       <c r="Z2" s="58"/>
       <c r="AA2" s="60"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="1:30" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
@@ -1799,11 +1800,11 @@
         <f>MAX(Y4:Y19)</f>
         <v>4</v>
       </c>
-      <c r="AC3"/>
-      <c r="AD3"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>1</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -1836,11 +1837,11 @@
         <v>-1</v>
       </c>
       <c r="AB4" s="14"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>2</v>
       </c>
       <c r="B5" s="21" t="s">
@@ -1873,11 +1874,11 @@
         <v>-1</v>
       </c>
       <c r="AB5" s="14"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="2"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -1907,11 +1908,11 @@
         <v>-2</v>
       </c>
       <c r="AB6" s="14"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="2"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>4</v>
       </c>
       <c r="B7" s="21" t="s">
@@ -1947,11 +1948,11 @@
         <v>0</v>
       </c>
       <c r="AB7" s="14"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="2"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>5</v>
       </c>
       <c r="B8" s="21" t="s">
@@ -1984,11 +1985,11 @@
         <v>-1</v>
       </c>
       <c r="AB8" s="14"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="2"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>6</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -2021,11 +2022,11 @@
         <v>-1</v>
       </c>
       <c r="AB9" s="14"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="2"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>7</v>
       </c>
       <c r="B10" s="21" t="s">
@@ -2055,11 +2056,11 @@
         <v>-2</v>
       </c>
       <c r="AB10" s="14"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="2"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>8</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -2092,11 +2093,11 @@
         <v>-1</v>
       </c>
       <c r="AB11" s="14"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="2"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>9</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -2128,11 +2129,11 @@
         <v>-1</v>
       </c>
       <c r="AB12" s="14"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="2"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>10</v>
       </c>
       <c r="B13" s="21" t="s">
@@ -2162,11 +2163,11 @@
         <v>-2</v>
       </c>
       <c r="AB13" s="14"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="2"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>11</v>
       </c>
       <c r="B14" s="21" t="s">
@@ -2198,11 +2199,11 @@
         <v>-1</v>
       </c>
       <c r="AB14" s="14"/>
-      <c r="AC14"/>
-      <c r="AD14"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="2"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>12</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -2232,11 +2233,11 @@
         <v>-2</v>
       </c>
       <c r="AB15" s="14"/>
-      <c r="AC15"/>
-      <c r="AD15"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="2"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>13</v>
       </c>
       <c r="B16" s="21" t="s">
@@ -2268,11 +2269,11 @@
         <v>-1</v>
       </c>
       <c r="AB16" s="14"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="2"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>14</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -2304,11 +2305,11 @@
         <v>-1</v>
       </c>
       <c r="AB17" s="14"/>
-      <c r="AC17"/>
-      <c r="AD17"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="2"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>15</v>
       </c>
       <c r="B18" s="21" t="s">
@@ -2340,11 +2341,11 @@
         <v>-1</v>
       </c>
       <c r="AB18" s="14"/>
-      <c r="AC18"/>
-      <c r="AD18"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="2"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>16</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -2377,8 +2378,8 @@
         <v>-1</v>
       </c>
       <c r="AB19" s="14"/>
-      <c r="AC19"/>
-      <c r="AD19"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="2"/>
     </row>
     <row r="20" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="22" t="s">
@@ -2413,11 +2414,11 @@
         <f>MAX(Y21:Y36)</f>
         <v>2</v>
       </c>
-      <c r="AC20"/>
-      <c r="AD20"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="2"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>1</v>
       </c>
       <c r="B21" s="57" t="s">
@@ -2447,11 +2448,11 @@
         <v>0</v>
       </c>
       <c r="AB21" s="14"/>
-      <c r="AC21"/>
-      <c r="AD21"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="2"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>2</v>
       </c>
       <c r="B22" s="57" t="s">
@@ -2481,11 +2482,11 @@
         <v>0</v>
       </c>
       <c r="AB22" s="14"/>
-      <c r="AC22"/>
-      <c r="AD22"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="2"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>3</v>
       </c>
       <c r="B23" s="57" t="s">
@@ -2515,11 +2516,11 @@
         <v>0</v>
       </c>
       <c r="AB23" s="14"/>
-      <c r="AC23"/>
-      <c r="AD23"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="2"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>4</v>
       </c>
       <c r="B24" s="57" t="s">
@@ -2549,11 +2550,11 @@
         <v>0</v>
       </c>
       <c r="AB24" s="14"/>
-      <c r="AC24"/>
-      <c r="AD24"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="2"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>5</v>
       </c>
       <c r="B25" s="57" t="s">
@@ -2583,11 +2584,11 @@
         <v>0</v>
       </c>
       <c r="AB25" s="14"/>
-      <c r="AC25"/>
-      <c r="AD25"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="2"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>6</v>
       </c>
       <c r="B26" s="57" t="s">
@@ -2617,11 +2618,11 @@
         <v>0</v>
       </c>
       <c r="AB26" s="14"/>
-      <c r="AC26"/>
-      <c r="AD26"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="2"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>7</v>
       </c>
       <c r="B27" s="57" t="s">
@@ -2651,11 +2652,11 @@
         <v>0</v>
       </c>
       <c r="AB27" s="14"/>
-      <c r="AC27"/>
-      <c r="AD27"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="2"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>8</v>
       </c>
       <c r="B28" s="57" t="s">
@@ -2682,11 +2683,11 @@
         <v>-1</v>
       </c>
       <c r="AB28" s="14"/>
-      <c r="AC28"/>
-      <c r="AD28"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="2"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>9</v>
       </c>
       <c r="B29" s="57" t="s">
@@ -2716,11 +2717,11 @@
         <v>0</v>
       </c>
       <c r="AB29" s="14"/>
-      <c r="AC29"/>
-      <c r="AD29"/>
+      <c r="AC29" s="6"/>
+      <c r="AD29" s="2"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="0">
         <v>10</v>
       </c>
       <c r="B30" s="57" t="s">
@@ -2750,11 +2751,11 @@
         <v>0</v>
       </c>
       <c r="AB30" s="14"/>
-      <c r="AC30"/>
-      <c r="AD30"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="2"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="0">
         <v>11</v>
       </c>
       <c r="B31" s="57" t="s">
@@ -2784,11 +2785,11 @@
         <v>0</v>
       </c>
       <c r="AB31" s="14"/>
-      <c r="AC31"/>
-      <c r="AD31"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="2"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="0">
         <v>12</v>
       </c>
       <c r="B32" s="57" t="s">
@@ -2818,11 +2819,11 @@
         <v>0</v>
       </c>
       <c r="AB32" s="14"/>
-      <c r="AC32"/>
-      <c r="AD32"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="2"/>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="0">
         <v>13</v>
       </c>
       <c r="B33" s="57" t="s">
@@ -2849,11 +2850,11 @@
         <v>-1</v>
       </c>
       <c r="AB33" s="14"/>
-      <c r="AC33"/>
-      <c r="AD33"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="2"/>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="0">
         <v>14</v>
       </c>
       <c r="B34" s="57" t="s">
@@ -2883,11 +2884,11 @@
         <v>0</v>
       </c>
       <c r="AB34" s="14"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="2"/>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="A35" s="0">
         <v>15</v>
       </c>
       <c r="B35" s="57" t="s">
@@ -2917,11 +2918,11 @@
         <v>0</v>
       </c>
       <c r="AB35" s="14"/>
-      <c r="AC35"/>
-      <c r="AD35"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="2"/>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="A36" s="0">
         <v>16</v>
       </c>
       <c r="B36" s="57" t="s">
@@ -2950,8 +2951,8 @@
         <v>0</v>
       </c>
       <c r="AB36" s="14"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="2"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B37" s="22" t="s">
@@ -2986,11 +2987,11 @@
         <f>MAX(Y38:Y53)</f>
         <v>2</v>
       </c>
-      <c r="AC37"/>
-      <c r="AD37"/>
+      <c r="AC37" s="6"/>
+      <c r="AD37" s="2"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="0">
         <v>1</v>
       </c>
       <c r="B38" s="57" t="s">
@@ -3020,11 +3021,11 @@
         <v>0</v>
       </c>
       <c r="AB38" s="14"/>
-      <c r="AC38"/>
-      <c r="AD38"/>
+      <c r="AC38" s="6"/>
+      <c r="AD38" s="2"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="0">
         <v>2</v>
       </c>
       <c r="B39" s="57" t="s">
@@ -3054,11 +3055,11 @@
         <v>0</v>
       </c>
       <c r="AB39" s="14"/>
-      <c r="AC39"/>
-      <c r="AD39"/>
+      <c r="AC39" s="6"/>
+      <c r="AD39" s="2"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="0">
         <v>3</v>
       </c>
       <c r="B40" s="57" t="s">
@@ -3087,11 +3088,11 @@
         <v>0</v>
       </c>
       <c r="AB40" s="14"/>
-      <c r="AC40"/>
-      <c r="AD40"/>
+      <c r="AC40" s="6"/>
+      <c r="AD40" s="2"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="0">
         <v>4</v>
       </c>
       <c r="B41" s="57" t="s">
@@ -3120,11 +3121,11 @@
         <v>0</v>
       </c>
       <c r="AB41" s="14"/>
-      <c r="AC41"/>
-      <c r="AD41"/>
+      <c r="AC41" s="6"/>
+      <c r="AD41" s="2"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="A42" s="0">
         <v>5</v>
       </c>
       <c r="B42" s="57" t="s">
@@ -3154,11 +3155,11 @@
         <v>0</v>
       </c>
       <c r="AB42" s="14"/>
-      <c r="AC42"/>
-      <c r="AD42"/>
+      <c r="AC42" s="6"/>
+      <c r="AD42" s="2"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="A43" s="0">
         <v>6</v>
       </c>
       <c r="B43" s="57" t="s">
@@ -3185,11 +3186,11 @@
         <v>-1</v>
       </c>
       <c r="AB43" s="14"/>
-      <c r="AC43"/>
-      <c r="AD43"/>
+      <c r="AC43" s="6"/>
+      <c r="AD43" s="2"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A44">
+      <c r="A44" s="0">
         <v>7</v>
       </c>
       <c r="B44" s="57" t="s">
@@ -3216,11 +3217,11 @@
         <v>-1</v>
       </c>
       <c r="AB44" s="14"/>
-      <c r="AC44"/>
-      <c r="AD44"/>
+      <c r="AC44" s="6"/>
+      <c r="AD44" s="2"/>
     </row>
     <row r="45" spans="1:30" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45">
+      <c r="A45" s="0">
         <v>8</v>
       </c>
       <c r="B45" s="57" t="s">
@@ -3247,11 +3248,11 @@
         <v>-1</v>
       </c>
       <c r="AB45" s="14"/>
-      <c r="AC45"/>
-      <c r="AD45"/>
+      <c r="AC45" s="6"/>
+      <c r="AD45" s="2"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A46">
+      <c r="A46" s="0">
         <v>9</v>
       </c>
       <c r="B46" s="57" t="s">
@@ -3278,11 +3279,11 @@
         <v>-1</v>
       </c>
       <c r="AB46" s="14"/>
-      <c r="AC46"/>
-      <c r="AD46"/>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="2"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A47">
+      <c r="A47" s="0">
         <v>10</v>
       </c>
       <c r="B47" s="57" t="s">
@@ -3309,11 +3310,11 @@
         <v>-1</v>
       </c>
       <c r="AB47" s="14"/>
-      <c r="AC47"/>
-      <c r="AD47"/>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="2"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A48">
+      <c r="A48" s="0">
         <v>11</v>
       </c>
       <c r="B48" s="57" t="s">
@@ -3340,11 +3341,11 @@
         <v>-1</v>
       </c>
       <c r="AB48" s="14"/>
-      <c r="AC48"/>
-      <c r="AD48"/>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="2"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="A49" s="0">
         <v>12</v>
       </c>
       <c r="B49" s="57" t="s">
@@ -3371,11 +3372,11 @@
         <v>-1</v>
       </c>
       <c r="AB49" s="14"/>
-      <c r="AC49"/>
-      <c r="AD49"/>
+      <c r="AC49" s="6"/>
+      <c r="AD49" s="2"/>
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="A50" s="0">
         <v>13</v>
       </c>
       <c r="B50" s="57" t="s">
@@ -3405,11 +3406,11 @@
         <v>0</v>
       </c>
       <c r="AB50" s="14"/>
-      <c r="AC50"/>
-      <c r="AD50"/>
+      <c r="AC50" s="6"/>
+      <c r="AD50" s="2"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="A51" s="0">
         <v>14</v>
       </c>
       <c r="B51" s="57" t="s">
@@ -3438,11 +3439,11 @@
         <v>0</v>
       </c>
       <c r="AB51" s="14"/>
-      <c r="AC51"/>
-      <c r="AD51"/>
+      <c r="AC51" s="6"/>
+      <c r="AD51" s="2"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A52">
+      <c r="A52" s="0">
         <v>15</v>
       </c>
       <c r="B52" s="57" t="s">
@@ -3469,11 +3470,11 @@
         <v>-1</v>
       </c>
       <c r="AB52" s="14"/>
-      <c r="AC52"/>
-      <c r="AD52"/>
+      <c r="AC52" s="6"/>
+      <c r="AD52" s="2"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A53">
+      <c r="A53" s="0">
         <v>16</v>
       </c>
       <c r="B53" s="57" t="s">
@@ -3500,8 +3501,8 @@
         <v>-1</v>
       </c>
       <c r="AB53" s="14"/>
-      <c r="AC53"/>
-      <c r="AD53"/>
+      <c r="AC53" s="6"/>
+      <c r="AD53" s="2"/>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="B54" s="22" t="s">
@@ -3536,11 +3537,11 @@
         <f>MAX(Y55:Y70)</f>
         <v>4</v>
       </c>
-      <c r="AC54"/>
-      <c r="AD54"/>
+      <c r="AC54" s="6"/>
+      <c r="AD54" s="2"/>
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A55">
+      <c r="A55" s="0">
         <v>1</v>
       </c>
       <c r="B55" s="56" t="s">
@@ -3573,11 +3574,11 @@
         <v>-1</v>
       </c>
       <c r="AB55" s="14"/>
-      <c r="AC55"/>
-      <c r="AD55"/>
+      <c r="AC55" s="6"/>
+      <c r="AD55" s="2"/>
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A56">
+      <c r="A56" s="0">
         <v>2</v>
       </c>
       <c r="B56" s="57" t="s">
@@ -3610,11 +3611,11 @@
         <v>-1</v>
       </c>
       <c r="AB56" s="14"/>
-      <c r="AC56"/>
-      <c r="AD56"/>
+      <c r="AC56" s="6"/>
+      <c r="AD56" s="2"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A57">
+      <c r="A57" s="0">
         <v>3</v>
       </c>
       <c r="B57" s="56" t="s">
@@ -3647,11 +3648,11 @@
         <v>-1</v>
       </c>
       <c r="AB57" s="14"/>
-      <c r="AC57"/>
-      <c r="AD57"/>
+      <c r="AC57" s="6"/>
+      <c r="AD57" s="2"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A58">
+      <c r="A58" s="0">
         <v>4</v>
       </c>
       <c r="B58" s="57" t="s">
@@ -3686,11 +3687,11 @@
         <v>0</v>
       </c>
       <c r="AB58" s="14"/>
-      <c r="AC58"/>
-      <c r="AD58"/>
+      <c r="AC58" s="6"/>
+      <c r="AD58" s="2"/>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A59">
+      <c r="A59" s="0">
         <v>5</v>
       </c>
       <c r="B59" s="57" t="s">
@@ -3723,11 +3724,11 @@
         <v>-1</v>
       </c>
       <c r="AB59" s="14"/>
-      <c r="AC59"/>
-      <c r="AD59"/>
+      <c r="AC59" s="6"/>
+      <c r="AD59" s="2"/>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A60">
+      <c r="A60" s="0">
         <v>6</v>
       </c>
       <c r="B60" s="56" t="s">
@@ -3760,11 +3761,11 @@
         <v>-1</v>
       </c>
       <c r="AB60" s="14"/>
-      <c r="AC60"/>
-      <c r="AD60"/>
+      <c r="AC60" s="6"/>
+      <c r="AD60" s="2"/>
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A61">
+      <c r="A61" s="0">
         <v>7</v>
       </c>
       <c r="B61" s="57" t="s">
@@ -3799,11 +3800,11 @@
         <v>0</v>
       </c>
       <c r="AB61" s="14"/>
-      <c r="AC61"/>
-      <c r="AD61"/>
+      <c r="AC61" s="6"/>
+      <c r="AD61" s="2"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A62">
+      <c r="A62" s="0">
         <v>8</v>
       </c>
       <c r="B62" s="56" t="s">
@@ -3839,11 +3840,11 @@
         <v>0</v>
       </c>
       <c r="AB62" s="14"/>
-      <c r="AC62"/>
-      <c r="AD62"/>
+      <c r="AC62" s="6"/>
+      <c r="AD62" s="2"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A63">
+      <c r="A63" s="0">
         <v>9</v>
       </c>
       <c r="B63" s="56" t="s">
@@ -3878,11 +3879,11 @@
         <v>0</v>
       </c>
       <c r="AB63" s="14"/>
-      <c r="AC63"/>
-      <c r="AD63"/>
+      <c r="AC63" s="6"/>
+      <c r="AD63" s="2"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A64">
+      <c r="A64" s="0">
         <v>10</v>
       </c>
       <c r="B64" s="57" t="s">
@@ -3918,11 +3919,11 @@
         <v>0</v>
       </c>
       <c r="AB64" s="14"/>
-      <c r="AC64"/>
-      <c r="AD64"/>
+      <c r="AC64" s="6"/>
+      <c r="AD64" s="2"/>
     </row>
     <row r="65" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A65">
+      <c r="A65" s="0">
         <v>11</v>
       </c>
       <c r="B65" s="56" t="s">
@@ -3952,11 +3953,11 @@
         <v>-2</v>
       </c>
       <c r="AB65" s="14"/>
-      <c r="AC65"/>
-      <c r="AD65"/>
+      <c r="AC65" s="6"/>
+      <c r="AD65" s="2"/>
     </row>
     <row r="66" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A66">
+      <c r="A66" s="0">
         <v>12</v>
       </c>
       <c r="B66" s="56" t="s">
@@ -3991,11 +3992,11 @@
         <v>0</v>
       </c>
       <c r="AB66" s="14"/>
-      <c r="AC66"/>
-      <c r="AD66"/>
+      <c r="AC66" s="6"/>
+      <c r="AD66" s="2"/>
     </row>
     <row r="67" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A67">
+      <c r="A67" s="0">
         <v>13</v>
       </c>
       <c r="B67" s="57" t="s">
@@ -4030,16 +4031,17 @@
         <v>0</v>
       </c>
       <c r="AB67" s="14"/>
-      <c r="AC67"/>
-      <c r="AD67"/>
+      <c r="AC67" s="6"/>
+      <c r="AD67" s="2"/>
     </row>
     <row r="68" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A68">
+      <c r="A68" s="0">
         <v>14</v>
       </c>
       <c r="B68" s="57" t="s">
         <v>77</v>
       </c>
+      <c r="H68" s="16"/>
       <c r="J68" s="17">
         <v>1</v>
       </c>
@@ -4050,28 +4052,28 @@
         <v>1</v>
       </c>
       <c r="W68" s="16"/>
-      <c r="X68" s="18">
+      <c r="X68" s="18" t="n">
         <f>SUM(C68:W68)</f>
-        <v>3</v>
-      </c>
-      <c r="Y68" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="Y68" s="19" t="n">
         <f>SUM(C68:W68)</f>
-        <v>3</v>
-      </c>
-      <c r="Z68" s="62">
+        <v>3.0</v>
+      </c>
+      <c r="Z68" s="62" t="n">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AA68" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="AA68" s="20" t="n">
         <f t="shared" si="7"/>
-        <v>-1</v>
+        <v>-1.0</v>
       </c>
       <c r="AB68" s="14"/>
-      <c r="AC68"/>
-      <c r="AD68"/>
+      <c r="AC68" s="6"/>
+      <c r="AD68" s="2"/>
     </row>
     <row r="69" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A69">
+      <c r="A69" s="0">
         <v>15</v>
       </c>
       <c r="B69" s="56" t="s">
@@ -4106,11 +4108,11 @@
         <v>0</v>
       </c>
       <c r="AB69" s="14"/>
-      <c r="AC69"/>
-      <c r="AD69"/>
+      <c r="AC69" s="6"/>
+      <c r="AD69" s="2"/>
     </row>
     <row r="70" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A70">
+      <c r="A70" s="0">
         <v>16</v>
       </c>
       <c r="B70" s="57" t="s">
@@ -4145,8 +4147,8 @@
         <v>0</v>
       </c>
       <c r="AB70" s="14"/>
-      <c r="AC70"/>
-      <c r="AD70"/>
+      <c r="AC70" s="6"/>
+      <c r="AD70" s="2"/>
     </row>
     <row r="71" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A71" s="26"/>
@@ -4174,24 +4176,24 @@
       <c r="U71" s="29"/>
       <c r="V71" s="29"/>
       <c r="W71" s="29"/>
-      <c r="X71" s="30">
+      <c r="X71" s="30" t="n">
         <f>SUM(X4:X70)</f>
-        <v>154</v>
-      </c>
-      <c r="Y71" s="31">
+        <v>154.0</v>
+      </c>
+      <c r="Y71" s="31" t="n">
         <f>SUM(Y4:Y70)</f>
-        <v>154</v>
-      </c>
-      <c r="AB71"/>
+        <v>154.0</v>
+      </c>
+      <c r="AB71" s="1"/>
     </row>
     <row r="72" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A72" s="26"/>
       <c r="B72" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C72" s="33">
+      <c r="C72" s="33" t="n">
         <f>SUM(X4:X19)</f>
-        <v>45</v>
+        <v>45.0</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
@@ -4215,16 +4217,16 @@
       <c r="W72" s="29"/>
       <c r="X72" s="34"/>
       <c r="Y72" s="26"/>
-      <c r="AB72"/>
+      <c r="AB72" s="1"/>
     </row>
     <row r="73" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A73" s="26"/>
       <c r="B73" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="33">
+      <c r="C73" s="33" t="n">
         <f>SUM(X21:X36)</f>
-        <v>30</v>
+        <v>30.0</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29"/>
@@ -4248,16 +4250,16 @@
       <c r="W73" s="29"/>
       <c r="X73" s="34"/>
       <c r="Y73" s="26"/>
-      <c r="AB73"/>
+      <c r="AB73" s="1"/>
     </row>
     <row r="74" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A74" s="26"/>
       <c r="B74" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C74" s="33">
+      <c r="C74" s="33" t="n">
         <f>SUM(X38:X53)</f>
-        <v>23</v>
+        <v>23.0</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29"/>
@@ -4281,16 +4283,16 @@
       <c r="W74" s="29"/>
       <c r="X74" s="34"/>
       <c r="Y74" s="26"/>
-      <c r="AB74"/>
+      <c r="AB74" s="1"/>
     </row>
     <row r="75" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A75" s="26"/>
       <c r="B75" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C75" s="35">
+      <c r="C75" s="35" t="n">
         <f>SUM(X55:X70)</f>
-        <v>56</v>
+        <v>56.0</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29"/>
@@ -4314,16 +4316,16 @@
       <c r="W75" s="29"/>
       <c r="X75" s="34"/>
       <c r="Y75" s="26"/>
-      <c r="AB75"/>
+      <c r="AB75" s="1"/>
     </row>
     <row r="76" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A76" s="26"/>
       <c r="B76" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C76" s="37">
+      <c r="C76" s="37" t="n">
         <f>SUM(C72:C75)</f>
-        <v>154</v>
+        <v>154.0</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29"/>
@@ -4347,7 +4349,7 @@
       <c r="W76" s="29"/>
       <c r="X76" s="34"/>
       <c r="Y76" s="26"/>
-      <c r="AB76"/>
+      <c r="AB76" s="1"/>
       <c r="AF76" s="26"/>
     </row>
     <row r="77" spans="1:42" x14ac:dyDescent="0.2">
@@ -4375,7 +4377,7 @@
       <c r="X77" s="39"/>
       <c r="Y77" s="38"/>
       <c r="Z77" s="40"/>
-      <c r="AB77"/>
+      <c r="AB77" s="1"/>
       <c r="AC77" s="41"/>
       <c r="AD77" s="42"/>
       <c r="AE77" s="26"/>
@@ -4416,7 +4418,7 @@
       <c r="X78" s="39"/>
       <c r="Y78" s="38"/>
       <c r="Z78" s="40"/>
-      <c r="AB78"/>
+      <c r="AB78" s="1"/>
       <c r="AC78" s="41"/>
       <c r="AD78" s="42"/>
       <c r="AE78" s="26"/>
@@ -4457,7 +4459,7 @@
       <c r="X79" s="39"/>
       <c r="Y79" s="38"/>
       <c r="Z79" s="40"/>
-      <c r="AB79"/>
+      <c r="AB79" s="1"/>
       <c r="AC79" s="41"/>
       <c r="AD79" s="42"/>
       <c r="AE79" s="26"/>
@@ -4498,7 +4500,7 @@
       <c r="X80" s="39"/>
       <c r="Y80" s="38"/>
       <c r="Z80" s="40"/>
-      <c r="AB80"/>
+      <c r="AB80" s="1"/>
       <c r="AC80" s="41"/>
       <c r="AD80" s="42"/>
       <c r="AE80" s="26"/>
@@ -4539,7 +4541,7 @@
       <c r="X81" s="39"/>
       <c r="Y81" s="38"/>
       <c r="Z81" s="40"/>
-      <c r="AB81"/>
+      <c r="AB81" s="1"/>
       <c r="AC81" s="41"/>
       <c r="AD81" s="42"/>
       <c r="AE81" s="26"/>
@@ -4580,7 +4582,7 @@
       <c r="X82" s="39"/>
       <c r="Y82" s="38"/>
       <c r="Z82" s="40"/>
-      <c r="AB82"/>
+      <c r="AB82" s="1"/>
       <c r="AC82" s="41"/>
       <c r="AD82" s="42"/>
       <c r="AE82" s="26"/>
@@ -4621,7 +4623,7 @@
       <c r="X83" s="39"/>
       <c r="Y83" s="38"/>
       <c r="Z83" s="40"/>
-      <c r="AB83"/>
+      <c r="AB83" s="1"/>
       <c r="AC83" s="41"/>
       <c r="AD83" s="42"/>
       <c r="AE83" s="26"/>
@@ -4662,7 +4664,7 @@
       <c r="X84" s="39"/>
       <c r="Y84" s="38"/>
       <c r="Z84" s="40"/>
-      <c r="AB84"/>
+      <c r="AB84" s="1"/>
       <c r="AC84" s="41"/>
       <c r="AD84" s="42"/>
       <c r="AE84" s="26"/>
@@ -4703,7 +4705,7 @@
       <c r="X85" s="39"/>
       <c r="Y85" s="38"/>
       <c r="Z85" s="40"/>
-      <c r="AB85"/>
+      <c r="AB85" s="1"/>
       <c r="AC85" s="41"/>
       <c r="AD85" s="42"/>
       <c r="AE85" s="26"/>
@@ -4744,7 +4746,7 @@
       <c r="X86" s="39"/>
       <c r="Y86" s="38"/>
       <c r="Z86" s="40"/>
-      <c r="AB86"/>
+      <c r="AB86" s="1"/>
       <c r="AC86" s="41"/>
       <c r="AD86" s="42"/>
       <c r="AE86" s="26"/>
@@ -4785,7 +4787,7 @@
       <c r="X87" s="39"/>
       <c r="Y87" s="38"/>
       <c r="Z87" s="40"/>
-      <c r="AB87"/>
+      <c r="AB87" s="1"/>
       <c r="AC87" s="41"/>
       <c r="AD87" s="42"/>
       <c r="AE87" s="26"/>
@@ -4826,7 +4828,7 @@
       <c r="X88" s="39"/>
       <c r="Y88" s="38"/>
       <c r="Z88" s="40"/>
-      <c r="AB88"/>
+      <c r="AB88" s="1"/>
       <c r="AC88" s="41"/>
       <c r="AD88" s="42"/>
       <c r="AE88" s="26"/>
@@ -4867,7 +4869,7 @@
       <c r="X89" s="39"/>
       <c r="Y89" s="38"/>
       <c r="Z89" s="40"/>
-      <c r="AB89"/>
+      <c r="AB89" s="1"/>
       <c r="AC89" s="41"/>
       <c r="AD89" s="42"/>
       <c r="AE89" s="26"/>
@@ -4908,7 +4910,7 @@
       <c r="X90" s="39"/>
       <c r="Y90" s="38"/>
       <c r="Z90" s="40"/>
-      <c r="AB90"/>
+      <c r="AB90" s="1"/>
       <c r="AC90" s="41"/>
       <c r="AD90" s="42"/>
       <c r="AE90" s="26"/>
@@ -4949,7 +4951,7 @@
       <c r="X91" s="39"/>
       <c r="Y91" s="38"/>
       <c r="Z91" s="40"/>
-      <c r="AB91"/>
+      <c r="AB91" s="1"/>
       <c r="AC91" s="41"/>
       <c r="AD91" s="42"/>
       <c r="AE91" s="26"/>
@@ -4990,7 +4992,7 @@
       <c r="X92" s="39"/>
       <c r="Y92" s="38"/>
       <c r="Z92" s="40"/>
-      <c r="AB92"/>
+      <c r="AB92" s="1"/>
       <c r="AC92" s="41"/>
       <c r="AD92" s="42"/>
       <c r="AE92" s="26"/>
@@ -5031,7 +5033,7 @@
       <c r="X93" s="39"/>
       <c r="Y93" s="38"/>
       <c r="Z93" s="40"/>
-      <c r="AB93"/>
+      <c r="AB93" s="1"/>
       <c r="AC93" s="41"/>
       <c r="AD93" s="42"/>
       <c r="AE93" s="26"/>
@@ -5072,7 +5074,7 @@
       <c r="X94" s="39"/>
       <c r="Y94" s="38"/>
       <c r="Z94" s="40"/>
-      <c r="AB94"/>
+      <c r="AB94" s="1"/>
       <c r="AC94" s="41"/>
       <c r="AD94" s="42"/>
       <c r="AE94" s="26"/>
@@ -5113,7 +5115,7 @@
       <c r="X95" s="39"/>
       <c r="Y95" s="38"/>
       <c r="Z95" s="40"/>
-      <c r="AB95"/>
+      <c r="AB95" s="1"/>
       <c r="AC95" s="41"/>
       <c r="AD95" s="42"/>
       <c r="AE95" s="26"/>
@@ -5154,7 +5156,7 @@
       <c r="X96" s="39"/>
       <c r="Y96" s="38"/>
       <c r="Z96" s="40"/>
-      <c r="AB96"/>
+      <c r="AB96" s="1"/>
       <c r="AC96" s="41"/>
       <c r="AD96" s="42"/>
       <c r="AE96" s="26"/>
@@ -5195,7 +5197,7 @@
       <c r="X97" s="39"/>
       <c r="Y97" s="38"/>
       <c r="Z97" s="40"/>
-      <c r="AB97"/>
+      <c r="AB97" s="1"/>
       <c r="AC97" s="41"/>
       <c r="AD97" s="42"/>
       <c r="AE97" s="26"/>
@@ -5236,7 +5238,7 @@
       <c r="X98" s="39"/>
       <c r="Y98" s="38"/>
       <c r="Z98" s="40"/>
-      <c r="AB98"/>
+      <c r="AB98" s="1"/>
       <c r="AC98" s="41"/>
       <c r="AD98" s="42"/>
       <c r="AE98" s="26"/>
@@ -5277,7 +5279,7 @@
       <c r="X99" s="39"/>
       <c r="Y99" s="38"/>
       <c r="Z99" s="40"/>
-      <c r="AB99"/>
+      <c r="AB99" s="1"/>
       <c r="AC99" s="41"/>
       <c r="AD99" s="42"/>
       <c r="AE99" s="26"/>
@@ -5318,7 +5320,7 @@
       <c r="X100" s="39"/>
       <c r="Y100" s="38"/>
       <c r="Z100" s="40"/>
-      <c r="AB100"/>
+      <c r="AB100" s="1"/>
       <c r="AC100" s="41"/>
       <c r="AD100" s="42"/>
       <c r="AE100" s="26"/>
@@ -5359,7 +5361,7 @@
       <c r="X101" s="39"/>
       <c r="Y101" s="38"/>
       <c r="Z101" s="40"/>
-      <c r="AB101"/>
+      <c r="AB101" s="1"/>
       <c r="AC101" s="41"/>
       <c r="AD101" s="42"/>
       <c r="AE101" s="26"/>
@@ -5400,7 +5402,7 @@
       <c r="X102" s="39"/>
       <c r="Y102" s="38"/>
       <c r="Z102" s="40"/>
-      <c r="AB102"/>
+      <c r="AB102" s="1"/>
       <c r="AC102" s="41"/>
       <c r="AD102" s="42"/>
       <c r="AE102" s="26"/>
@@ -5441,7 +5443,7 @@
       <c r="X103" s="39"/>
       <c r="Y103" s="38"/>
       <c r="Z103" s="40"/>
-      <c r="AB103"/>
+      <c r="AB103" s="1"/>
       <c r="AC103" s="41"/>
       <c r="AD103" s="42"/>
       <c r="AE103" s="26"/>
@@ -5482,7 +5484,7 @@
       <c r="X104" s="39"/>
       <c r="Y104" s="38"/>
       <c r="Z104" s="40"/>
-      <c r="AB104"/>
+      <c r="AB104" s="1"/>
       <c r="AC104" s="41"/>
       <c r="AD104" s="42"/>
       <c r="AE104" s="26"/>
@@ -5523,7 +5525,7 @@
       <c r="X105" s="39"/>
       <c r="Y105" s="38"/>
       <c r="Z105" s="40"/>
-      <c r="AB105"/>
+      <c r="AB105" s="1"/>
       <c r="AC105" s="41"/>
       <c r="AD105" s="42"/>
       <c r="AE105" s="26"/>
@@ -5564,7 +5566,7 @@
       <c r="X106" s="39"/>
       <c r="Y106" s="38"/>
       <c r="Z106" s="40"/>
-      <c r="AB106"/>
+      <c r="AB106" s="1"/>
       <c r="AC106" s="41"/>
       <c r="AD106" s="42"/>
       <c r="AE106" s="26"/>
@@ -5605,7 +5607,7 @@
       <c r="X107" s="39"/>
       <c r="Y107" s="38"/>
       <c r="Z107" s="40"/>
-      <c r="AB107"/>
+      <c r="AB107" s="1"/>
       <c r="AC107" s="41"/>
       <c r="AD107" s="42"/>
       <c r="AE107" s="26"/>
@@ -5646,7 +5648,7 @@
       <c r="X108" s="39"/>
       <c r="Y108" s="38"/>
       <c r="Z108" s="40"/>
-      <c r="AB108"/>
+      <c r="AB108" s="1"/>
       <c r="AC108" s="41"/>
       <c r="AD108" s="42"/>
       <c r="AE108" s="26"/>
@@ -5687,7 +5689,7 @@
       <c r="X109" s="39"/>
       <c r="Y109" s="38"/>
       <c r="Z109" s="40"/>
-      <c r="AB109"/>
+      <c r="AB109" s="1"/>
       <c r="AC109" s="41"/>
       <c r="AD109" s="42"/>
       <c r="AE109" s="26"/>
@@ -5728,7 +5730,7 @@
       <c r="X110" s="39"/>
       <c r="Y110" s="38"/>
       <c r="Z110" s="40"/>
-      <c r="AB110"/>
+      <c r="AB110" s="1"/>
       <c r="AC110" s="41"/>
       <c r="AD110" s="42"/>
       <c r="AE110" s="26"/>
@@ -5769,7 +5771,7 @@
       <c r="X111" s="39"/>
       <c r="Y111" s="38"/>
       <c r="Z111" s="40"/>
-      <c r="AB111"/>
+      <c r="AB111" s="1"/>
       <c r="AC111" s="41"/>
       <c r="AD111" s="42"/>
       <c r="AE111" s="26"/>
@@ -5810,7 +5812,7 @@
       <c r="X112" s="39"/>
       <c r="Y112" s="38"/>
       <c r="Z112" s="40"/>
-      <c r="AB112"/>
+      <c r="AB112" s="1"/>
       <c r="AC112" s="41"/>
       <c r="AD112" s="42"/>
       <c r="AE112" s="26"/>
@@ -5851,7 +5853,7 @@
       <c r="X113" s="39"/>
       <c r="Y113" s="38"/>
       <c r="Z113" s="40"/>
-      <c r="AB113"/>
+      <c r="AB113" s="1"/>
       <c r="AC113" s="41"/>
       <c r="AD113" s="42"/>
       <c r="AE113" s="26"/>
@@ -5892,7 +5894,7 @@
       <c r="X114" s="39"/>
       <c r="Y114" s="38"/>
       <c r="Z114" s="40"/>
-      <c r="AB114"/>
+      <c r="AB114" s="1"/>
       <c r="AC114" s="41"/>
       <c r="AD114" s="42"/>
       <c r="AE114" s="26"/>
@@ -5933,7 +5935,7 @@
       <c r="X115" s="39"/>
       <c r="Y115" s="38"/>
       <c r="Z115" s="40"/>
-      <c r="AB115"/>
+      <c r="AB115" s="1"/>
       <c r="AC115" s="41"/>
       <c r="AD115" s="42"/>
       <c r="AE115" s="26"/>
@@ -5974,7 +5976,7 @@
       <c r="X116" s="39"/>
       <c r="Y116" s="38"/>
       <c r="Z116" s="40"/>
-      <c r="AB116"/>
+      <c r="AB116" s="1"/>
       <c r="AC116" s="41"/>
       <c r="AD116" s="42"/>
       <c r="AE116" s="26"/>
@@ -6015,7 +6017,7 @@
       <c r="X117" s="39"/>
       <c r="Y117" s="38"/>
       <c r="Z117" s="40"/>
-      <c r="AB117"/>
+      <c r="AB117" s="1"/>
       <c r="AC117" s="41"/>
       <c r="AD117" s="42"/>
       <c r="AE117" s="26"/>
@@ -6056,7 +6058,7 @@
       <c r="X118" s="39"/>
       <c r="Y118" s="38"/>
       <c r="Z118" s="40"/>
-      <c r="AB118"/>
+      <c r="AB118" s="1"/>
       <c r="AC118" s="41"/>
       <c r="AD118" s="42"/>
       <c r="AE118" s="26"/>
@@ -6097,7 +6099,7 @@
       <c r="X119" s="39"/>
       <c r="Y119" s="38"/>
       <c r="Z119" s="40"/>
-      <c r="AB119"/>
+      <c r="AB119" s="1"/>
       <c r="AC119" s="41"/>
       <c r="AD119" s="42"/>
       <c r="AE119" s="26"/>
@@ -6138,7 +6140,7 @@
       <c r="X120" s="39"/>
       <c r="Y120" s="38"/>
       <c r="Z120" s="40"/>
-      <c r="AB120"/>
+      <c r="AB120" s="1"/>
       <c r="AC120" s="41"/>
       <c r="AD120" s="42"/>
       <c r="AE120" s="26"/>
@@ -6179,7 +6181,7 @@
       <c r="X121" s="39"/>
       <c r="Y121" s="38"/>
       <c r="Z121" s="40"/>
-      <c r="AB121"/>
+      <c r="AB121" s="1"/>
       <c r="AC121" s="41"/>
       <c r="AD121" s="42"/>
       <c r="AE121" s="26"/>
@@ -6220,7 +6222,7 @@
       <c r="X122" s="44"/>
       <c r="Y122" s="43"/>
       <c r="Z122" s="26"/>
-      <c r="AB122"/>
+      <c r="AB122" s="1"/>
       <c r="AC122" s="41"/>
       <c r="AD122" s="42"/>
       <c r="AE122" s="26"/>
@@ -6261,7 +6263,7 @@
       <c r="X123" s="46"/>
       <c r="Y123" s="45"/>
       <c r="Z123" s="26"/>
-      <c r="AB123"/>
+      <c r="AB123" s="1"/>
       <c r="AC123" s="41"/>
       <c r="AD123" s="42"/>
       <c r="AE123" s="26"/>
@@ -6302,7 +6304,7 @@
       <c r="X124" s="46"/>
       <c r="Y124" s="45"/>
       <c r="Z124" s="26"/>
-      <c r="AB124"/>
+      <c r="AB124" s="1"/>
       <c r="AC124" s="41"/>
       <c r="AD124" s="42"/>
       <c r="AE124" s="26"/>
@@ -6343,7 +6345,7 @@
       <c r="X125" s="46"/>
       <c r="Y125" s="45"/>
       <c r="Z125" s="26"/>
-      <c r="AB125"/>
+      <c r="AB125" s="1"/>
       <c r="AC125" s="41"/>
       <c r="AD125" s="42"/>
       <c r="AE125" s="26"/>
@@ -6384,7 +6386,7 @@
       <c r="X126" s="46"/>
       <c r="Y126" s="45"/>
       <c r="Z126" s="26"/>
-      <c r="AB126"/>
+      <c r="AB126" s="1"/>
       <c r="AC126" s="41"/>
       <c r="AD126" s="42"/>
       <c r="AE126" s="26"/>
@@ -6425,7 +6427,7 @@
       <c r="X127" s="46"/>
       <c r="Y127" s="45"/>
       <c r="Z127" s="26"/>
-      <c r="AB127"/>
+      <c r="AB127" s="1"/>
       <c r="AC127" s="41"/>
       <c r="AD127" s="42"/>
       <c r="AE127" s="26"/>
@@ -6466,7 +6468,7 @@
       <c r="X128" s="46"/>
       <c r="Y128" s="45"/>
       <c r="Z128" s="26"/>
-      <c r="AB128"/>
+      <c r="AB128" s="1"/>
       <c r="AC128" s="41"/>
       <c r="AD128" s="42"/>
       <c r="AE128" s="26"/>
@@ -6507,7 +6509,7 @@
       <c r="X129" s="46"/>
       <c r="Y129" s="45"/>
       <c r="Z129" s="26"/>
-      <c r="AB129"/>
+      <c r="AB129" s="1"/>
       <c r="AC129" s="41"/>
       <c r="AD129" s="42"/>
       <c r="AE129" s="26"/>
@@ -6548,7 +6550,7 @@
       <c r="X130" s="46"/>
       <c r="Y130" s="45"/>
       <c r="Z130" s="26"/>
-      <c r="AB130"/>
+      <c r="AB130" s="1"/>
       <c r="AC130" s="41"/>
       <c r="AD130" s="42"/>
       <c r="AE130" s="26"/>
@@ -6589,7 +6591,7 @@
       <c r="X131" s="46"/>
       <c r="Y131" s="45"/>
       <c r="Z131" s="26"/>
-      <c r="AB131"/>
+      <c r="AB131" s="1"/>
       <c r="AC131" s="41"/>
       <c r="AD131" s="42"/>
       <c r="AE131" s="26"/>
@@ -6630,7 +6632,7 @@
       <c r="X132" s="46"/>
       <c r="Y132" s="45"/>
       <c r="Z132" s="26"/>
-      <c r="AB132"/>
+      <c r="AB132" s="1"/>
       <c r="AC132" s="41"/>
       <c r="AD132" s="42"/>
       <c r="AE132" s="26"/>
@@ -6671,7 +6673,7 @@
       <c r="X133" s="46"/>
       <c r="Y133" s="45"/>
       <c r="Z133" s="26"/>
-      <c r="AB133"/>
+      <c r="AB133" s="1"/>
       <c r="AC133" s="41"/>
       <c r="AD133" s="42"/>
       <c r="AE133" s="26"/>
@@ -6712,7 +6714,7 @@
       <c r="X134" s="46"/>
       <c r="Y134" s="45"/>
       <c r="Z134" s="26"/>
-      <c r="AB134"/>
+      <c r="AB134" s="1"/>
       <c r="AC134" s="41"/>
       <c r="AD134" s="42"/>
       <c r="AE134" s="26"/>
@@ -6753,7 +6755,7 @@
       <c r="X135" s="46"/>
       <c r="Y135" s="45"/>
       <c r="Z135" s="26"/>
-      <c r="AB135"/>
+      <c r="AB135" s="1"/>
       <c r="AC135" s="41"/>
       <c r="AD135" s="42"/>
       <c r="AE135" s="26"/>
@@ -6794,7 +6796,7 @@
       <c r="X136" s="46"/>
       <c r="Y136" s="45"/>
       <c r="Z136" s="26"/>
-      <c r="AB136"/>
+      <c r="AB136" s="1"/>
       <c r="AC136" s="41"/>
       <c r="AD136" s="42"/>
       <c r="AE136" s="26"/>
@@ -6810,124 +6812,124 @@
       <c r="AP136" s="26"/>
     </row>
     <row r="137" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB137"/>
+      <c r="AB137" s="1"/>
     </row>
     <row r="138" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB138"/>
+      <c r="AB138" s="1"/>
     </row>
     <row r="139" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB139"/>
+      <c r="AB139" s="1"/>
     </row>
     <row r="140" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB140"/>
+      <c r="AB140" s="1"/>
     </row>
     <row r="141" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB141"/>
+      <c r="AB141" s="1"/>
     </row>
     <row r="142" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB142"/>
+      <c r="AB142" s="1"/>
     </row>
     <row r="143" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB143"/>
+      <c r="AB143" s="1"/>
     </row>
     <row r="144" spans="3:42" x14ac:dyDescent="0.2">
-      <c r="AB144"/>
+      <c r="AB144" s="1"/>
     </row>
     <row r="145" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB145"/>
+      <c r="AB145" s="1"/>
     </row>
     <row r="146" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB146"/>
+      <c r="AB146" s="1"/>
     </row>
     <row r="147" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB147"/>
+      <c r="AB147" s="1"/>
     </row>
     <row r="148" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB148"/>
+      <c r="AB148" s="1"/>
     </row>
     <row r="149" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB149"/>
+      <c r="AB149" s="1"/>
     </row>
     <row r="150" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB150"/>
+      <c r="AB150" s="1"/>
     </row>
     <row r="151" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB151"/>
+      <c r="AB151" s="1"/>
     </row>
     <row r="152" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB152"/>
+      <c r="AB152" s="1"/>
     </row>
     <row r="153" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB153"/>
+      <c r="AB153" s="1"/>
     </row>
     <row r="154" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB154"/>
+      <c r="AB154" s="1"/>
     </row>
     <row r="155" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB155"/>
+      <c r="AB155" s="1"/>
     </row>
     <row r="156" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB156"/>
+      <c r="AB156" s="1"/>
     </row>
     <row r="157" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB157"/>
+      <c r="AB157" s="1"/>
     </row>
     <row r="158" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB158"/>
+      <c r="AB158" s="1"/>
     </row>
     <row r="159" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB159"/>
+      <c r="AB159" s="1"/>
     </row>
     <row r="160" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB160"/>
+      <c r="AB160" s="1"/>
     </row>
     <row r="161" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB161"/>
+      <c r="AB161" s="1"/>
     </row>
     <row r="162" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB162"/>
+      <c r="AB162" s="1"/>
     </row>
     <row r="163" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB163"/>
+      <c r="AB163" s="1"/>
     </row>
     <row r="164" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB164"/>
+      <c r="AB164" s="1"/>
     </row>
     <row r="165" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB165"/>
+      <c r="AB165" s="1"/>
     </row>
     <row r="166" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB166"/>
+      <c r="AB166" s="1"/>
     </row>
     <row r="167" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB167"/>
+      <c r="AB167" s="1"/>
     </row>
     <row r="168" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB168"/>
+      <c r="AB168" s="1"/>
     </row>
     <row r="169" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB169"/>
+      <c r="AB169" s="1"/>
     </row>
     <row r="170" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB170"/>
+      <c r="AB170" s="1"/>
     </row>
     <row r="171" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB171"/>
+      <c r="AB171" s="1"/>
     </row>
     <row r="172" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB172"/>
+      <c r="AB172" s="1"/>
     </row>
     <row r="173" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB173"/>
+      <c r="AB173" s="1"/>
     </row>
     <row r="174" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB174"/>
+      <c r="AB174" s="1"/>
     </row>
     <row r="175" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB175"/>
+      <c r="AB175" s="1"/>
     </row>
     <row r="176" spans="28:28" x14ac:dyDescent="0.2">
-      <c r="AB176"/>
+      <c r="AB176" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>